<commit_message>
Singleton, repository pattern and  class for memento(not finished)
</commit_message>
<xml_diff>
--- a/Appointment.xlsx
+++ b/Appointment.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Stomatolog</t>
   </si>
@@ -38,28 +38,22 @@
     <t>Ora Data</t>
   </si>
   <si>
-    <t>Andrian</t>
+    <t>Iulia</t>
   </si>
   <si>
-    <t>dafaa</t>
+    <t>12:00</t>
   </si>
   <si>
-    <t>daffsdf</t>
+    <t>03847474</t>
   </si>
   <si>
-    <t>16:00</t>
+    <t>Înălbire</t>
   </si>
   <si>
-    <t>06674574</t>
+    <t>5/24/2024</t>
   </si>
   <si>
-    <t>Tratarea cariei</t>
-  </si>
-  <si>
-    <t>5/16/2024</t>
-  </si>
-  <si>
-    <t>16:005/16/2024</t>
+    <t>12:005/24/2024</t>
   </si>
 </sst>
 </file>
@@ -143,25 +137,25 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Memento(saving works, restoring not yet))
</commit_message>
<xml_diff>
--- a/Appointment.xlsx
+++ b/Appointment.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Stomatolog</t>
   </si>
@@ -38,22 +38,28 @@
     <t>Ora Data</t>
   </si>
   <si>
-    <t>Iulia</t>
+    <t>Andrei</t>
   </si>
   <si>
-    <t>12:00</t>
+    <t>Valeriu</t>
   </si>
   <si>
-    <t>03847474</t>
+    <t>Darius</t>
   </si>
   <si>
-    <t>Înălbire</t>
+    <t>15:00</t>
   </si>
   <si>
-    <t>5/24/2024</t>
+    <t>084756374</t>
   </si>
   <si>
-    <t>12:005/24/2024</t>
+    <t>Extracție</t>
+  </si>
+  <si>
+    <t>5/29/2024</t>
+  </si>
+  <si>
+    <t>15:005/29/2024</t>
   </si>
 </sst>
 </file>
@@ -137,25 +143,25 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Memento is working and now deleting data from database more consistent
</commit_message>
<xml_diff>
--- a/Appointment.xlsx
+++ b/Appointment.xlsx
@@ -38,28 +38,28 @@
     <t>Ora Data</t>
   </si>
   <si>
-    <t>Andrei</t>
+    <t>Andrian</t>
   </si>
   <si>
-    <t>Valeriu</t>
+    <t>Jock</t>
   </si>
   <si>
-    <t>Darius</t>
+    <t>Dock</t>
   </si>
   <si>
-    <t>15:00</t>
+    <t>13:00</t>
   </si>
   <si>
-    <t>084756374</t>
+    <t>043764635645</t>
   </si>
   <si>
-    <t>Extracție</t>
+    <t>Tratarea cariei</t>
   </si>
   <si>
-    <t>5/29/2024</t>
+    <t>5/23/2024</t>
   </si>
   <si>
-    <t>15:005/29/2024</t>
+    <t>13:005/23/2024</t>
   </si>
 </sst>
 </file>

</xml_diff>